<commit_message>
Create Migration & setup UI
- Create Migration untuk tabel data, sektor, wilayah
- Setup view Layout.app2
</commit_message>
<xml_diff>
--- a/datasample.xlsx
+++ b/datasample.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KPI\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\dashborpdb\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0575E140-E061-4FE8-A586-E8095ED31983}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16770" windowHeight="6945"/>
+    <workbookView xWindow="22932" yWindow="5508" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -385,16 +386,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -408,7 +409,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -422,7 +423,7 @@
         <v>-6309865</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -436,7 +437,7 @@
         <v>-1422264</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -450,7 +451,7 @@
         <v>-72840</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -464,7 +465,7 @@
         <v>-878862</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -478,7 +479,7 @@
         <v>-4190</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -492,7 +493,7 @@
         <v>-259280</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -506,7 +507,7 @@
         <v>-430177</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -520,7 +521,7 @@
         <v>-199029</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -534,7 +535,7 @@
         <v>-4769</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -548,7 +549,7 @@
         <v>-2270524</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -562,7 +563,7 @@
         <v>-707250</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -576,7 +577,7 @@
         <v>-785293</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -590,7 +591,7 @@
         <v>-531828</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -604,7 +605,7 @@
         <v>-1596</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -618,7 +619,7 @@
         <v>-68447</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -632,7 +633,7 @@
         <v>-1578688</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>

</xml_diff>